<commit_message>
Refining alignment tree structure and logic
</commit_message>
<xml_diff>
--- a/tabular/virus/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/virus/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452FB58A-1AFD-D64A-B496-055666B5B5E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -19,23 +13,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$121</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="821">
   <si>
     <t>AY632538</t>
   </si>
@@ -2503,7 +2497,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2771,7 +2765,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="718">
+  <cellStyleXfs count="725">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3392,6 +3386,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3642,7 +3643,7 @@
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="718">
+  <cellStyles count="725">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4050,6 +4051,13 @@
     <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4696,15 +4704,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" style="1" customWidth="1"/>
@@ -4721,7 +4729,7 @@
     <col min="14" max="14" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="19">
       <c r="A1" s="9" t="s">
         <v>213</v>
       </c>
@@ -4765,7 +4773,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>251</v>
       </c>
@@ -4807,7 +4815,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>280</v>
       </c>
@@ -4849,7 +4857,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>282</v>
       </c>
@@ -4891,7 +4899,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="18" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
@@ -4933,7 +4941,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="18" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
@@ -4975,7 +4983,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="18" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>240</v>
       </c>
@@ -5017,7 +5025,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>273</v>
       </c>
@@ -5059,7 +5067,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="18" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>255</v>
       </c>
@@ -5101,7 +5109,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="18" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>639</v>
       </c>
@@ -5143,7 +5151,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -5185,7 +5193,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="18" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -5227,7 +5235,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="18" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>272</v>
       </c>
@@ -5269,7 +5277,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="18" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>248</v>
       </c>
@@ -5311,7 +5319,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="18" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>640</v>
       </c>
@@ -5353,7 +5361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="18" customHeight="1">
       <c r="A16" s="64" t="s">
         <v>764</v>
       </c>
@@ -5393,7 +5401,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="18" customHeight="1">
       <c r="A17" s="64" t="s">
         <v>765</v>
       </c>
@@ -5433,7 +5441,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="18" customHeight="1">
       <c r="A18" s="64" t="s">
         <v>767</v>
       </c>
@@ -5473,7 +5481,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="18" customHeight="1">
       <c r="A19" s="72" t="s">
         <v>805</v>
       </c>
@@ -5511,7 +5519,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="18" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>196</v>
       </c>
@@ -5553,7 +5561,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="18" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>17</v>
       </c>
@@ -5595,7 +5603,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="18" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>11</v>
       </c>
@@ -5637,7 +5645,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="18" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>35</v>
       </c>
@@ -5679,7 +5687,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="18" customHeight="1">
       <c r="A24" s="21" t="s">
         <v>252</v>
       </c>
@@ -5721,7 +5729,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="18" customHeight="1">
       <c r="A25" s="19" t="s">
         <v>26</v>
       </c>
@@ -5763,7 +5771,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="18" customHeight="1">
       <c r="A26" s="19" t="s">
         <v>39</v>
       </c>
@@ -5805,7 +5813,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="18" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>41</v>
       </c>
@@ -5847,7 +5855,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="18" customHeight="1">
       <c r="A28" s="24" t="s">
         <v>19</v>
       </c>
@@ -5889,7 +5897,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="18" customHeight="1">
       <c r="A29" s="27" t="s">
         <v>274</v>
       </c>
@@ -5931,7 +5939,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="18" customHeight="1">
       <c r="A30" s="29" t="s">
         <v>3</v>
       </c>
@@ -5973,7 +5981,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="18" customHeight="1">
       <c r="A31" s="32" t="s">
         <v>247</v>
       </c>
@@ -6015,7 +6023,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="18" customHeight="1">
       <c r="A32" s="29" t="s">
         <v>15</v>
       </c>
@@ -6057,7 +6065,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="18" customHeight="1">
       <c r="A33" s="32" t="s">
         <v>283</v>
       </c>
@@ -6099,7 +6107,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="18" customHeight="1">
       <c r="A34" s="32" t="s">
         <v>268</v>
       </c>
@@ -6141,7 +6149,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="18" customHeight="1">
       <c r="A35" s="32" t="s">
         <v>219</v>
       </c>
@@ -6183,7 +6191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="18" customHeight="1">
       <c r="A36" s="32" t="s">
         <v>277</v>
       </c>
@@ -6225,7 +6233,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="18" customHeight="1">
       <c r="A37" s="32" t="s">
         <v>278</v>
       </c>
@@ -6267,7 +6275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="18" customHeight="1">
       <c r="A38" s="32" t="s">
         <v>226</v>
       </c>
@@ -6309,7 +6317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="18" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>0</v>
       </c>
@@ -6351,7 +6359,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="18" customHeight="1">
       <c r="A40" s="32" t="s">
         <v>284</v>
       </c>
@@ -6393,7 +6401,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="18" customHeight="1">
       <c r="A41" s="32" t="s">
         <v>217</v>
       </c>
@@ -6433,7 +6441,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="18" customHeight="1">
       <c r="A42" s="32" t="s">
         <v>246</v>
       </c>
@@ -6475,7 +6483,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="18" customHeight="1">
       <c r="A43" s="29" t="s">
         <v>7</v>
       </c>
@@ -6517,7 +6525,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="18" customHeight="1">
       <c r="A44" s="32" t="s">
         <v>216</v>
       </c>
@@ -6559,7 +6567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="18" customHeight="1">
       <c r="A45" s="32" t="s">
         <v>276</v>
       </c>
@@ -6601,7 +6609,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="18" customHeight="1">
       <c r="A46" s="29" t="s">
         <v>8</v>
       </c>
@@ -6643,7 +6651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="18" customHeight="1">
       <c r="A47" s="32" t="s">
         <v>288</v>
       </c>
@@ -6685,7 +6693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="18" customHeight="1">
       <c r="A48" s="29" t="s">
         <v>2</v>
       </c>
@@ -6727,7 +6735,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="18" customHeight="1">
       <c r="A49" s="32" t="s">
         <v>275</v>
       </c>
@@ -6769,7 +6777,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="18" customHeight="1">
       <c r="A50" s="32" t="s">
         <v>281</v>
       </c>
@@ -6811,7 +6819,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="18" customHeight="1">
       <c r="A51" s="29" t="s">
         <v>14</v>
       </c>
@@ -6853,7 +6861,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="18" customHeight="1">
       <c r="A52" s="32" t="s">
         <v>285</v>
       </c>
@@ -6895,7 +6903,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="18" customHeight="1">
       <c r="A53" s="29" t="s">
         <v>16</v>
       </c>
@@ -6937,7 +6945,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="18" customHeight="1">
       <c r="A54" s="32" t="s">
         <v>241</v>
       </c>
@@ -6979,7 +6987,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="18" customHeight="1">
       <c r="A55" s="32" t="s">
         <v>279</v>
       </c>
@@ -7021,7 +7029,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="18" customHeight="1">
       <c r="A56" s="29" t="s">
         <v>6</v>
       </c>
@@ -7063,7 +7071,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="18" customHeight="1">
       <c r="A57" s="32" t="s">
         <v>245</v>
       </c>
@@ -7105,7 +7113,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="18" customHeight="1">
       <c r="A58" s="32" t="s">
         <v>688</v>
       </c>
@@ -7147,7 +7155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="18" customHeight="1">
       <c r="A59" s="32" t="s">
         <v>689</v>
       </c>
@@ -7189,7 +7197,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="18" customHeight="1">
       <c r="A60" s="32" t="s">
         <v>690</v>
       </c>
@@ -7231,7 +7239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="18" customHeight="1">
       <c r="A61" s="32" t="s">
         <v>691</v>
       </c>
@@ -7273,7 +7281,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="18" customHeight="1">
       <c r="A62" s="32" t="s">
         <v>692</v>
       </c>
@@ -7315,7 +7323,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="18" customHeight="1">
       <c r="A63" s="32" t="s">
         <v>693</v>
       </c>
@@ -7357,7 +7365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="18" customHeight="1">
       <c r="A64" s="32" t="s">
         <v>695</v>
       </c>
@@ -7399,7 +7407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="18" customHeight="1">
       <c r="A65" s="35" t="s">
         <v>5</v>
       </c>
@@ -7441,7 +7449,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="18" customHeight="1">
       <c r="A66" s="35" t="s">
         <v>54</v>
       </c>
@@ -7483,7 +7491,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="18" customHeight="1">
       <c r="A67" s="35" t="s">
         <v>53</v>
       </c>
@@ -7525,7 +7533,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="18" customHeight="1">
       <c r="A68" s="35" t="s">
         <v>57</v>
       </c>
@@ -7567,7 +7575,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="18" customHeight="1">
       <c r="A69" s="35" t="s">
         <v>55</v>
       </c>
@@ -7609,7 +7617,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="18" customHeight="1">
       <c r="A70" s="35" t="s">
         <v>244</v>
       </c>
@@ -7651,7 +7659,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="18" customHeight="1">
       <c r="A71" s="35" t="s">
         <v>56</v>
       </c>
@@ -7693,7 +7701,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="18" customHeight="1">
       <c r="A72" s="35" t="s">
         <v>249</v>
       </c>
@@ -7735,7 +7743,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="18" customHeight="1">
       <c r="A73" s="35" t="s">
         <v>224</v>
       </c>
@@ -7777,7 +7785,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="18" customHeight="1">
       <c r="A74" s="35" t="s">
         <v>694</v>
       </c>
@@ -7819,7 +7827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="18" customHeight="1">
       <c r="A75" s="37" t="s">
         <v>230</v>
       </c>
@@ -7861,7 +7869,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="18" customHeight="1">
       <c r="A76" s="37" t="s">
         <v>267</v>
       </c>
@@ -7903,7 +7911,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="18" customHeight="1">
       <c r="A77" s="37" t="s">
         <v>228</v>
       </c>
@@ -7945,7 +7953,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="18" customHeight="1">
       <c r="A78" s="37" t="s">
         <v>237</v>
       </c>
@@ -7987,7 +7995,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="18" customHeight="1">
       <c r="A79" s="37" t="s">
         <v>229</v>
       </c>
@@ -8029,7 +8037,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="18" customHeight="1">
       <c r="A80" s="37" t="s">
         <v>644</v>
       </c>
@@ -8071,7 +8079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="18" customHeight="1">
       <c r="A81" s="40" t="s">
         <v>243</v>
       </c>
@@ -8113,7 +8121,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="18" customHeight="1">
       <c r="A82" s="40" t="s">
         <v>269</v>
       </c>
@@ -8155,7 +8163,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="19">
       <c r="A83" s="40" t="s">
         <v>238</v>
       </c>
@@ -8197,7 +8205,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="19">
       <c r="A84" s="74" t="s">
         <v>820</v>
       </c>
@@ -8239,7 +8247,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="19">
       <c r="A85" s="42" t="s">
         <v>59</v>
       </c>
@@ -8281,7 +8289,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="19">
       <c r="A86" s="42" t="s">
         <v>60</v>
       </c>
@@ -8323,7 +8331,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="19">
       <c r="A87" s="42" t="s">
         <v>260</v>
       </c>
@@ -8365,7 +8373,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="19">
       <c r="A88" s="42" t="s">
         <v>215</v>
       </c>
@@ -8407,7 +8415,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="18" customHeight="1">
       <c r="A89" s="42" t="s">
         <v>234</v>
       </c>
@@ -8449,7 +8457,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="18" customHeight="1">
       <c r="A90" s="42" t="s">
         <v>222</v>
       </c>
@@ -8491,7 +8499,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="18" customHeight="1">
       <c r="A91" s="42" t="s">
         <v>58</v>
       </c>
@@ -8533,7 +8541,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="18" customHeight="1">
       <c r="A92" s="42" t="s">
         <v>239</v>
       </c>
@@ -8575,7 +8583,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="19">
       <c r="A93" s="42" t="s">
         <v>233</v>
       </c>
@@ -8617,7 +8625,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="19">
       <c r="A94" s="42" t="s">
         <v>214</v>
       </c>
@@ -8659,7 +8667,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="19">
       <c r="A95" s="42" t="s">
         <v>61</v>
       </c>
@@ -8701,7 +8709,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="19">
       <c r="A96" s="42" t="s">
         <v>271</v>
       </c>
@@ -8743,7 +8751,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="19">
       <c r="A97" s="42" t="s">
         <v>220</v>
       </c>
@@ -8785,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="19">
       <c r="A98" s="42" t="s">
         <v>4</v>
       </c>
@@ -8827,7 +8835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="19">
       <c r="A99" s="42" t="s">
         <v>259</v>
       </c>
@@ -8869,7 +8877,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="19">
       <c r="A100" s="55" t="s">
         <v>218</v>
       </c>
@@ -8911,7 +8919,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="19">
       <c r="A101" s="55" t="s">
         <v>225</v>
       </c>
@@ -8953,7 +8961,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="19">
       <c r="A102" s="55" t="s">
         <v>227</v>
       </c>
@@ -8995,7 +9003,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="19">
       <c r="A103" s="55" t="s">
         <v>232</v>
       </c>
@@ -9037,7 +9045,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="19">
       <c r="A104" s="55" t="s">
         <v>286</v>
       </c>
@@ -9079,7 +9087,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="19">
       <c r="A105" s="55" t="s">
         <v>258</v>
       </c>
@@ -9121,7 +9129,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="19">
       <c r="A106" s="55" t="s">
         <v>231</v>
       </c>
@@ -9163,7 +9171,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="19">
       <c r="A107" s="55" t="s">
         <v>250</v>
       </c>
@@ -9205,7 +9213,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="19">
       <c r="A108" s="55" t="s">
         <v>253</v>
       </c>
@@ -9247,7 +9255,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="19">
       <c r="A109" s="55" t="s">
         <v>265</v>
       </c>
@@ -9289,7 +9297,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="19">
       <c r="A110" s="55" t="s">
         <v>655</v>
       </c>
@@ -9331,7 +9339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="19">
       <c r="A111" s="55" t="s">
         <v>667</v>
       </c>
@@ -9371,7 +9379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="19">
       <c r="A112" s="55" t="s">
         <v>554</v>
       </c>
@@ -9413,7 +9421,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="19">
       <c r="A113" s="55" t="s">
         <v>482</v>
       </c>
@@ -9455,7 +9463,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="19">
       <c r="A114" s="55" t="s">
         <v>487</v>
       </c>
@@ -9497,7 +9505,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="19">
       <c r="A115" s="55" t="s">
         <v>631</v>
       </c>
@@ -9537,7 +9545,7 @@
       </c>
       <c r="N115" s="54"/>
     </row>
-    <row r="116" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="19">
       <c r="A116" s="55" t="s">
         <v>785</v>
       </c>
@@ -9568,7 +9576,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="19">
       <c r="A117" s="55" t="s">
         <v>787</v>
       </c>
@@ -9599,7 +9607,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="19">
       <c r="A118" s="55" t="s">
         <v>791</v>
       </c>
@@ -9630,7 +9638,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="19">
       <c r="A119" s="55" t="s">
         <v>793</v>
       </c>
@@ -9664,7 +9672,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="19">
       <c r="A120" s="55" t="s">
         <v>615</v>
       </c>
@@ -9706,7 +9714,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="19">
       <c r="A121" s="55" t="s">
         <v>616</v>
       </c>
@@ -9748,7 +9756,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="19">
       <c r="A122" s="55" t="s">
         <v>789</v>
       </c>
@@ -9779,7 +9787,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="19">
       <c r="A123" s="55" t="s">
         <v>763</v>
       </c>
@@ -9811,7 +9819,7 @@
       </c>
       <c r="L123" s="59"/>
     </row>
-    <row r="124" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="19">
       <c r="A124" s="55" t="s">
         <v>766</v>
       </c>
@@ -9842,7 +9850,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="19">
       <c r="A125" s="55" t="s">
         <v>235</v>
       </c>
@@ -9884,7 +9892,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="19">
       <c r="A126" s="55" t="s">
         <v>497</v>
       </c>
@@ -9924,7 +9932,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="19">
       <c r="A127" s="55" t="s">
         <v>495</v>
       </c>
@@ -9964,7 +9972,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="19">
       <c r="A128" s="55" t="s">
         <v>496</v>
       </c>
@@ -10004,7 +10012,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="18">
       <c r="A129" s="55" t="s">
         <v>555</v>
       </c>
@@ -10021,9 +10029,11 @@
         <v>670</v>
       </c>
       <c r="F129" s="70" t="s">
+        <v>483</v>
+      </c>
+      <c r="G129" s="70" t="s">
         <v>797</v>
       </c>
-      <c r="G129" s="68"/>
       <c r="H129" s="68"/>
       <c r="I129" s="68" t="s">
         <v>564</v>
@@ -10044,7 +10054,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="18">
       <c r="A130" s="55" t="s">
         <v>553</v>
       </c>
@@ -10061,9 +10071,11 @@
         <v>670</v>
       </c>
       <c r="F130" s="70" t="s">
+        <v>483</v>
+      </c>
+      <c r="G130" s="70" t="s">
         <v>797</v>
       </c>
-      <c r="G130" s="68"/>
       <c r="H130" s="68"/>
       <c r="I130" s="68" t="s">
         <v>560</v>
@@ -10084,7 +10096,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="19">
       <c r="A131" s="27" t="s">
         <v>236</v>
       </c>
@@ -10124,7 +10136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="19">
       <c r="A132" s="27" t="s">
         <v>270</v>
       </c>
@@ -10164,7 +10176,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="19">
       <c r="A133" s="27" t="s">
         <v>262</v>
       </c>
@@ -10204,7 +10216,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="19">
       <c r="A134" s="27" t="s">
         <v>263</v>
       </c>
@@ -10244,7 +10256,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="19">
       <c r="A135" s="27" t="s">
         <v>264</v>
       </c>
@@ -10284,7 +10296,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="19">
       <c r="A136" s="27" t="s">
         <v>256</v>
       </c>
@@ -10324,7 +10336,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="19">
       <c r="A137" s="27" t="s">
         <v>678</v>
       </c>
@@ -10361,7 +10373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="19">
       <c r="A138" s="27" t="s">
         <v>679</v>
       </c>
@@ -10398,7 +10410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="19">
       <c r="A139" s="27" t="s">
         <v>680</v>
       </c>
@@ -10435,7 +10447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="19">
       <c r="A140" s="27" t="s">
         <v>681</v>
       </c>
@@ -10472,7 +10484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="19">
       <c r="A141" s="27" t="s">
         <v>682</v>
       </c>
@@ -10509,7 +10521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="19">
       <c r="A142" s="27" t="s">
         <v>683</v>
       </c>
@@ -10546,7 +10558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="19">
       <c r="A143" s="27" t="s">
         <v>684</v>
       </c>
@@ -10583,7 +10595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="19">
       <c r="A144" s="27" t="s">
         <v>687</v>
       </c>
@@ -10620,7 +10632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="19">
       <c r="A145" s="27" t="s">
         <v>686</v>
       </c>
@@ -10660,7 +10672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="19">
       <c r="A146" s="27" t="s">
         <v>254</v>
       </c>
@@ -10700,7 +10712,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="19">
       <c r="A147" s="27" t="s">
         <v>221</v>
       </c>
@@ -10740,7 +10752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="19">
       <c r="A148" s="27" t="s">
         <v>287</v>
       </c>
@@ -10780,7 +10792,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="19">
       <c r="A149" s="27" t="s">
         <v>266</v>
       </c>
@@ -10820,7 +10832,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="19">
       <c r="A150" s="27" t="s">
         <v>223</v>
       </c>
@@ -10860,7 +10872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="19">
       <c r="A151" s="27" t="s">
         <v>257</v>
       </c>
@@ -10900,7 +10912,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="19">
       <c r="A152" s="27" t="s">
         <v>261</v>
       </c>
@@ -10940,7 +10952,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="19">
       <c r="A153" s="27" t="s">
         <v>685</v>
       </c>
@@ -10980,7 +10992,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="19">
       <c r="A154" s="48" t="s">
         <v>570</v>
       </c>
@@ -11024,7 +11036,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="19">
       <c r="A155" s="48" t="s">
         <v>568</v>
       </c>
@@ -11068,7 +11080,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="19">
       <c r="A156" s="48" t="s">
         <v>567</v>
       </c>
@@ -11112,7 +11124,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="19">
       <c r="A157" s="48" t="s">
         <v>661</v>
       </c>
@@ -11156,7 +11168,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="19">
       <c r="A158" s="48" t="s">
         <v>569</v>
       </c>
@@ -11200,7 +11212,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="19">
       <c r="A159" s="48" t="s">
         <v>635</v>
       </c>
@@ -11244,7 +11256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="19">
       <c r="A160" s="48" t="s">
         <v>638</v>
       </c>
@@ -11288,7 +11300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="19">
       <c r="A161" s="48" t="s">
         <v>662</v>
       </c>
@@ -11332,7 +11344,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="19">
       <c r="A162" s="48" t="s">
         <v>814</v>
       </c>
@@ -11373,7 +11385,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="19">
       <c r="A163" s="48" t="s">
         <v>815</v>
       </c>
@@ -11414,7 +11426,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="19">
       <c r="A164" s="48" t="s">
         <v>816</v>
       </c>
@@ -11455,18 +11467,18 @@
         <v>577</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14">
       <c r="A165" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N161">
+  <sortState ref="A2:N161">
     <sortCondition ref="D2:D161"/>
     <sortCondition ref="E2:E161"/>
     <sortCondition ref="F2:F161"/>
     <sortCondition ref="G2:G161"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B61" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B61" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11479,16 +11491,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>617</v>
       </c>
@@ -11520,7 +11532,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="19">
       <c r="A2" s="42" t="s">
         <v>242</v>
       </c>

</xml_diff>

<commit_message>
Jingmen tick virus represented as a concatemer of segment1 and segment3
</commit_message>
<xml_diff>
--- a/tabular/virus/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/virus/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/virus/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE21B36-76C7-AD40-9B38-C4CC0C61C4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="34680" windowHeight="20940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -13,23 +19,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flavi.txt!$A$1:$M$121</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="819">
   <si>
     <t>AY632538</t>
   </si>
@@ -2050,12 +2050,6 @@
     <t>RHCV</t>
   </si>
   <si>
-    <t>JMTV1</t>
-  </si>
-  <si>
-    <t>JMTV3</t>
-  </si>
-  <si>
     <t>Jingmenvirus</t>
   </si>
   <si>
@@ -2314,9 +2308,6 @@
     <t>HepaPegi</t>
   </si>
   <si>
-    <t>Hepegivirus</t>
-  </si>
-  <si>
     <t>Gammarus chevreuxi flavivirus</t>
   </si>
   <si>
@@ -2492,12 +2483,15 @@
   </si>
   <si>
     <t>KJ152564</t>
+  </si>
+  <si>
+    <t>JMTV_CONCAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2592,7 +2586,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2709,12 +2703,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -3492,7 +3480,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3622,26 +3610,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="725">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4704,15 +4689,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N165"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" style="1" customWidth="1"/>
@@ -4729,7 +4714,7 @@
     <col min="14" max="14" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19">
+    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>213</v>
       </c>
@@ -4740,7 +4725,7 @@
         <v>62</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>668</v>
@@ -4773,7 +4758,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1">
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>251</v>
       </c>
@@ -4784,7 +4769,7 @@
         <v>410</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>670</v>
@@ -4815,7 +4800,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1">
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>280</v>
       </c>
@@ -4826,7 +4811,7 @@
         <v>342</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>670</v>
@@ -4857,7 +4842,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1">
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>282</v>
       </c>
@@ -4868,7 +4853,7 @@
         <v>384</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>670</v>
@@ -4899,7 +4884,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1">
+    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
@@ -4910,7 +4895,7 @@
         <v>314</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>670</v>
@@ -4941,7 +4926,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1">
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
@@ -4952,7 +4937,7 @@
         <v>316</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>670</v>
@@ -4983,7 +4968,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>240</v>
       </c>
@@ -4994,7 +4979,7 @@
         <v>209</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>670</v>
@@ -5025,7 +5010,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1">
+    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>273</v>
       </c>
@@ -5036,7 +5021,7 @@
         <v>436</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>670</v>
@@ -5067,7 +5052,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1">
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>255</v>
       </c>
@@ -5078,7 +5063,7 @@
         <v>614</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>670</v>
@@ -5109,7 +5094,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1">
+    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>639</v>
       </c>
@@ -5120,7 +5105,7 @@
         <v>311</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>670</v>
@@ -5151,7 +5136,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1">
+    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>36</v>
       </c>
@@ -5162,7 +5147,7 @@
         <v>423</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>670</v>
@@ -5193,7 +5178,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1">
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -5204,7 +5189,7 @@
         <v>319</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>670</v>
@@ -5235,7 +5220,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1">
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>272</v>
       </c>
@@ -5246,7 +5231,7 @@
         <v>434</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>670</v>
@@ -5277,7 +5262,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1">
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>248</v>
       </c>
@@ -5288,7 +5273,7 @@
         <v>405</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>670</v>
@@ -5319,7 +5304,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>640</v>
       </c>
@@ -5330,7 +5315,7 @@
         <v>669</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>670</v>
@@ -5361,165 +5346,165 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1">
-      <c r="A16" s="64" t="s">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="63" t="s">
+        <v>761</v>
+      </c>
+      <c r="B16" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>771</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>747</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>670</v>
+      </c>
+      <c r="F16" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="64" t="s">
+        <v>774</v>
+      </c>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64" t="s">
+        <v>775</v>
+      </c>
+      <c r="J16" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="K16" s="64"/>
+      <c r="L16" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="63" t="s">
+        <v>762</v>
+      </c>
+      <c r="B17" s="64" t="s">
+        <v>766</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>772</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>747</v>
+      </c>
+      <c r="E17" s="64" t="s">
+        <v>670</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="64" t="s">
+        <v>774</v>
+      </c>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64" t="s">
+        <v>776</v>
+      </c>
+      <c r="J17" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="K17" s="64"/>
+      <c r="L17" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
         <v>764</v>
       </c>
-      <c r="B16" s="65" t="s">
-        <v>762</v>
-      </c>
-      <c r="C16" s="65" t="s">
+      <c r="B18" s="64" t="s">
+        <v>768</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>773</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>747</v>
+      </c>
+      <c r="E18" s="64" t="s">
+        <v>670</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" s="64" t="s">
         <v>774</v>
       </c>
-      <c r="D16" s="65" t="s">
-        <v>749</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>670</v>
-      </c>
-      <c r="F16" s="65" t="s">
+      <c r="H18" s="64"/>
+      <c r="I18" s="64" t="s">
+        <v>775</v>
+      </c>
+      <c r="J18" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="K18" s="64"/>
+      <c r="L18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="71" t="s">
+        <v>802</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>796</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>797</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>747</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>670</v>
+      </c>
+      <c r="F19" s="70" t="s">
         <v>191</v>
       </c>
-      <c r="G16" s="65" t="s">
-        <v>777</v>
-      </c>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65" t="s">
-        <v>778</v>
-      </c>
-      <c r="J16" s="65" t="s">
-        <v>780</v>
-      </c>
-      <c r="K16" s="65"/>
-      <c r="L16" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1">
-      <c r="A17" s="64" t="s">
-        <v>765</v>
-      </c>
-      <c r="B17" s="65" t="s">
-        <v>769</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>775</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>749</v>
-      </c>
-      <c r="E17" s="65" t="s">
-        <v>670</v>
-      </c>
-      <c r="F17" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="G17" s="65" t="s">
-        <v>777</v>
-      </c>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65" t="s">
-        <v>779</v>
-      </c>
-      <c r="J17" s="65" t="s">
-        <v>780</v>
-      </c>
-      <c r="K17" s="65"/>
-      <c r="L17" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1">
-      <c r="A18" s="64" t="s">
-        <v>767</v>
-      </c>
-      <c r="B18" s="65" t="s">
-        <v>771</v>
-      </c>
-      <c r="C18" s="65" t="s">
-        <v>776</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>749</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>670</v>
-      </c>
-      <c r="F18" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="G18" s="65" t="s">
-        <v>777</v>
-      </c>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65" t="s">
-        <v>778</v>
-      </c>
-      <c r="J18" s="65" t="s">
-        <v>780</v>
-      </c>
-      <c r="K18" s="65"/>
-      <c r="L18" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" s="16" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1">
-      <c r="A19" s="72" t="s">
-        <v>805</v>
-      </c>
-      <c r="B19" s="71" t="s">
+      <c r="G19" s="70" t="s">
+        <v>798</v>
+      </c>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70" t="s">
         <v>799</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="J19" s="70" t="s">
         <v>800</v>
       </c>
-      <c r="D19" s="71" t="s">
-        <v>749</v>
-      </c>
-      <c r="E19" s="71" t="s">
-        <v>670</v>
-      </c>
-      <c r="F19" s="71" t="s">
-        <v>191</v>
-      </c>
-      <c r="G19" s="71" t="s">
-        <v>801</v>
-      </c>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71" t="s">
-        <v>802</v>
-      </c>
-      <c r="J19" s="71" t="s">
-        <v>803</v>
-      </c>
-      <c r="K19" s="71" t="s">
-        <v>803</v>
+      <c r="K19" s="70" t="s">
+        <v>800</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
       <c r="N19" s="16" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>196</v>
       </c>
@@ -5530,7 +5515,7 @@
         <v>328</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>670</v>
@@ -5561,7 +5546,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1">
+    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>17</v>
       </c>
@@ -5572,7 +5557,7 @@
         <v>326</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>670</v>
@@ -5603,7 +5588,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1">
+    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>11</v>
       </c>
@@ -5614,7 +5599,7 @@
         <v>318</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>670</v>
@@ -5623,7 +5608,7 @@
         <v>191</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20" t="s">
@@ -5645,7 +5630,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1">
+    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>35</v>
       </c>
@@ -5656,7 +5641,7 @@
         <v>420</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>670</v>
@@ -5665,7 +5650,7 @@
         <v>191</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="23" t="s">
@@ -5687,7 +5672,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1">
+    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>252</v>
       </c>
@@ -5698,7 +5683,7 @@
         <v>414</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>670</v>
@@ -5707,7 +5692,7 @@
         <v>191</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="23" t="s">
@@ -5729,7 +5714,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1">
+    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>26</v>
       </c>
@@ -5737,10 +5722,10 @@
         <v>140</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>670</v>
@@ -5749,7 +5734,7 @@
         <v>191</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="23" t="s">
@@ -5771,7 +5756,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1">
+    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>39</v>
       </c>
@@ -5782,7 +5767,7 @@
         <v>424</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>670</v>
@@ -5791,7 +5776,7 @@
         <v>191</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H26" s="23"/>
       <c r="I26" s="23" t="s">
@@ -5813,7 +5798,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1">
+    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>41</v>
       </c>
@@ -5824,7 +5809,7 @@
         <v>425</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>670</v>
@@ -5833,7 +5818,7 @@
         <v>191</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H27" s="23"/>
       <c r="I27" s="23" t="s">
@@ -5855,7 +5840,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1">
+    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>19</v>
       </c>
@@ -5866,7 +5851,7 @@
         <v>329</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>670</v>
@@ -5897,7 +5882,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="18" customHeight="1">
+    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>274</v>
       </c>
@@ -5908,7 +5893,7 @@
         <v>438</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>670</v>
@@ -5939,7 +5924,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18" customHeight="1">
+    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
         <v>3</v>
       </c>
@@ -5950,7 +5935,7 @@
         <v>293</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>670</v>
@@ -5981,7 +5966,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18" customHeight="1">
+    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>247</v>
       </c>
@@ -5992,7 +5977,7 @@
         <v>402</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>670</v>
@@ -6023,7 +6008,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="18" customHeight="1">
+    <row r="32" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
         <v>15</v>
       </c>
@@ -6034,7 +6019,7 @@
         <v>588</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>670</v>
@@ -6065,7 +6050,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18" customHeight="1">
+    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>283</v>
       </c>
@@ -6076,7 +6061,7 @@
         <v>393</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>670</v>
@@ -6107,7 +6092,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18" customHeight="1">
+    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
         <v>268</v>
       </c>
@@ -6118,7 +6103,7 @@
         <v>428</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>670</v>
@@ -6149,7 +6134,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>219</v>
       </c>
@@ -6160,7 +6145,7 @@
         <v>339</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>670</v>
@@ -6191,7 +6176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18" customHeight="1">
+    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>277</v>
       </c>
@@ -6202,7 +6187,7 @@
         <v>336</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>670</v>
@@ -6233,7 +6218,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
         <v>278</v>
       </c>
@@ -6244,7 +6229,7 @@
         <v>337</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>670</v>
@@ -6275,7 +6260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>226</v>
       </c>
@@ -6286,7 +6271,7 @@
         <v>206</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>670</v>
@@ -6317,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1">
+    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>0</v>
       </c>
@@ -6328,7 +6313,7 @@
         <v>289</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>670</v>
@@ -6356,10 +6341,10 @@
         <v>476</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>284</v>
       </c>
@@ -6370,7 +6355,7 @@
         <v>395</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>670</v>
@@ -6401,7 +6386,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18" customHeight="1">
+    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
         <v>217</v>
       </c>
@@ -6412,7 +6397,7 @@
         <v>473</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>670</v>
@@ -6441,7 +6426,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18" customHeight="1">
+    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>246</v>
       </c>
@@ -6452,7 +6437,7 @@
         <v>399</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>670</v>
@@ -6483,7 +6468,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1">
+    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>7</v>
       </c>
@@ -6494,7 +6479,7 @@
         <v>306</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>670</v>
@@ -6525,7 +6510,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1">
+    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>216</v>
       </c>
@@ -6536,7 +6521,7 @@
         <v>331</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>670</v>
@@ -6567,7 +6552,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="18" customHeight="1">
+    <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
         <v>276</v>
       </c>
@@ -6578,7 +6563,7 @@
         <v>445</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>670</v>
@@ -6609,7 +6594,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="18" customHeight="1">
+    <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>8</v>
       </c>
@@ -6620,7 +6605,7 @@
         <v>309</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E46" s="30" t="s">
         <v>670</v>
@@ -6651,7 +6636,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="18" customHeight="1">
+    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
         <v>288</v>
       </c>
@@ -6662,7 +6647,7 @@
         <v>415</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>670</v>
@@ -6693,7 +6678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1">
+    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
         <v>2</v>
       </c>
@@ -6704,7 +6689,7 @@
         <v>291</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>670</v>
@@ -6735,7 +6720,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1">
+    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
         <v>275</v>
       </c>
@@ -6746,7 +6731,7 @@
         <v>439</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>670</v>
@@ -6777,7 +6762,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1">
+    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>281</v>
       </c>
@@ -6788,7 +6773,7 @@
         <v>383</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>670</v>
@@ -6819,7 +6804,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1">
+    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
         <v>14</v>
       </c>
@@ -6830,7 +6815,7 @@
         <v>320</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>670</v>
@@ -6861,7 +6846,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1">
+    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
         <v>285</v>
       </c>
@@ -6872,7 +6857,7 @@
         <v>412</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>670</v>
@@ -6903,7 +6888,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1">
+    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
         <v>16</v>
       </c>
@@ -6914,7 +6899,7 @@
         <v>589</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>670</v>
@@ -6945,7 +6930,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1">
+    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
         <v>241</v>
       </c>
@@ -6956,7 +6941,7 @@
         <v>377</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>670</v>
@@ -6987,7 +6972,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1">
+    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
         <v>279</v>
       </c>
@@ -6998,7 +6983,7 @@
         <v>203</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>670</v>
@@ -7029,7 +7014,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1">
+    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
         <v>6</v>
       </c>
@@ -7040,7 +7025,7 @@
         <v>303</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>670</v>
@@ -7071,7 +7056,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1">
+    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
         <v>245</v>
       </c>
@@ -7082,7 +7067,7 @@
         <v>397</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>670</v>
@@ -7113,18 +7098,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1">
+    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D58" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E58" s="33" t="s">
         <v>670</v>
@@ -7146,7 +7131,7 @@
         <v>629</v>
       </c>
       <c r="L58" s="59" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="M58" s="13" t="s">
         <v>1</v>
@@ -7155,18 +7140,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1">
+    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B59" s="33" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D59" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E59" s="33" t="s">
         <v>670</v>
@@ -7188,27 +7173,27 @@
         <v>629</v>
       </c>
       <c r="L59" s="59" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="M59" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N59" s="59" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D60" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E60" s="33" t="s">
         <v>670</v>
@@ -7239,18 +7224,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1">
+    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E61" s="33" t="s">
         <v>670</v>
@@ -7278,21 +7263,21 @@
         <v>1</v>
       </c>
       <c r="N61" s="59" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B62" s="33" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D62" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E62" s="33" t="s">
         <v>670</v>
@@ -7320,21 +7305,21 @@
         <v>1</v>
       </c>
       <c r="N62" s="59" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C63" s="33" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D63" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E63" s="33" t="s">
         <v>670</v>
@@ -7356,7 +7341,7 @@
         <v>630</v>
       </c>
       <c r="L63" s="59" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="M63" s="13" t="s">
         <v>1</v>
@@ -7365,18 +7350,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1">
+    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C64" s="33" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D64" s="33" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E64" s="33" t="s">
         <v>670</v>
@@ -7398,7 +7383,7 @@
         <v>629</v>
       </c>
       <c r="L64" s="59" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="M64" s="13" t="s">
         <v>1</v>
@@ -7407,7 +7392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="18" customHeight="1">
+    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
         <v>5</v>
       </c>
@@ -7418,7 +7403,7 @@
         <v>301</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E65" s="36" t="s">
         <v>670</v>
@@ -7449,7 +7434,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="18" customHeight="1">
+    <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
         <v>54</v>
       </c>
@@ -7460,7 +7445,7 @@
         <v>448</v>
       </c>
       <c r="D66" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E66" s="36" t="s">
         <v>670</v>
@@ -7491,7 +7476,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="18" customHeight="1">
+    <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
         <v>53</v>
       </c>
@@ -7502,7 +7487,7 @@
         <v>442</v>
       </c>
       <c r="D67" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E67" s="36" t="s">
         <v>670</v>
@@ -7533,7 +7518,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="18" customHeight="1">
+    <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="35" t="s">
         <v>57</v>
       </c>
@@ -7544,7 +7529,7 @@
         <v>455</v>
       </c>
       <c r="D68" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E68" s="36" t="s">
         <v>670</v>
@@ -7575,7 +7560,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="18" customHeight="1">
+    <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
         <v>55</v>
       </c>
@@ -7586,7 +7571,7 @@
         <v>451</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E69" s="36" t="s">
         <v>670</v>
@@ -7617,7 +7602,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="18" customHeight="1">
+    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
         <v>244</v>
       </c>
@@ -7628,7 +7613,7 @@
         <v>389</v>
       </c>
       <c r="D70" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E70" s="36" t="s">
         <v>670</v>
@@ -7659,7 +7644,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="18" customHeight="1">
+    <row r="71" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>56</v>
       </c>
@@ -7670,7 +7655,7 @@
         <v>453</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E71" s="36" t="s">
         <v>670</v>
@@ -7701,7 +7686,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="18" customHeight="1">
+    <row r="72" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="35" t="s">
         <v>249</v>
       </c>
@@ -7712,7 +7697,7 @@
         <v>406</v>
       </c>
       <c r="D72" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E72" s="36" t="s">
         <v>670</v>
@@ -7743,7 +7728,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="18" customHeight="1">
+    <row r="73" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="35" t="s">
         <v>224</v>
       </c>
@@ -7754,7 +7739,7 @@
         <v>205</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E73" s="36" t="s">
         <v>670</v>
@@ -7785,18 +7770,18 @@
         <v>565</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="18" customHeight="1">
+    <row r="74" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="35" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C74" s="36" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D74" s="36" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E74" s="36" t="s">
         <v>670</v>
@@ -7818,7 +7803,7 @@
         <v>630</v>
       </c>
       <c r="L74" s="59" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="M74" s="13" t="s">
         <v>1</v>
@@ -7827,7 +7812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="18" customHeight="1">
+    <row r="75" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="37" t="s">
         <v>230</v>
       </c>
@@ -7838,7 +7823,7 @@
         <v>358</v>
       </c>
       <c r="D75" s="38" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E75" s="38" t="s">
         <v>670</v>
@@ -7869,7 +7854,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="18" customHeight="1">
+    <row r="76" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="37" t="s">
         <v>267</v>
       </c>
@@ -7880,7 +7865,7 @@
         <v>426</v>
       </c>
       <c r="D76" s="38" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E76" s="38" t="s">
         <v>670</v>
@@ -7911,7 +7896,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="18" customHeight="1">
+    <row r="77" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="37" t="s">
         <v>228</v>
       </c>
@@ -7922,7 +7907,7 @@
         <v>353</v>
       </c>
       <c r="D77" s="38" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E77" s="38" t="s">
         <v>670</v>
@@ -7953,7 +7938,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="18" customHeight="1">
+    <row r="78" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="37" t="s">
         <v>237</v>
       </c>
@@ -7964,7 +7949,7 @@
         <v>369</v>
       </c>
       <c r="D78" s="38" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E78" s="38" t="s">
         <v>670</v>
@@ -7995,7 +7980,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="18" customHeight="1">
+    <row r="79" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="37" t="s">
         <v>229</v>
       </c>
@@ -8006,7 +7991,7 @@
         <v>355</v>
       </c>
       <c r="D79" s="38" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E79" s="38" t="s">
         <v>670</v>
@@ -8037,7 +8022,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="18" customHeight="1">
+    <row r="80" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="37" t="s">
         <v>644</v>
       </c>
@@ -8048,7 +8033,7 @@
         <v>646</v>
       </c>
       <c r="D80" s="38" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E80" s="38" t="s">
         <v>670</v>
@@ -8079,7 +8064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="18" customHeight="1">
+    <row r="81" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="40" t="s">
         <v>243</v>
       </c>
@@ -8090,7 +8075,7 @@
         <v>386</v>
       </c>
       <c r="D81" s="41" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E81" s="41" t="s">
         <v>670</v>
@@ -8121,7 +8106,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="18" customHeight="1">
+    <row r="82" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="40" t="s">
         <v>269</v>
       </c>
@@ -8132,7 +8117,7 @@
         <v>431</v>
       </c>
       <c r="D82" s="41" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E82" s="41" t="s">
         <v>670</v>
@@ -8163,7 +8148,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="19">
+    <row r="83" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A83" s="40" t="s">
         <v>238</v>
       </c>
@@ -8174,7 +8159,7 @@
         <v>372</v>
       </c>
       <c r="D83" s="41" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E83" s="41" t="s">
         <v>670</v>
@@ -8205,36 +8190,36 @@
         <v>537</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="19">
-      <c r="A84" s="74" t="s">
-        <v>820</v>
-      </c>
-      <c r="B84" s="73" t="s">
-        <v>819</v>
-      </c>
-      <c r="C84" s="73" t="s">
+    <row r="84" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A84" s="73" t="s">
+        <v>817</v>
+      </c>
+      <c r="B84" s="72" t="s">
+        <v>816</v>
+      </c>
+      <c r="C84" s="72" t="s">
         <v>438</v>
       </c>
-      <c r="D84" s="73" t="s">
-        <v>749</v>
-      </c>
-      <c r="E84" s="73" t="s">
-        <v>670</v>
-      </c>
-      <c r="F84" s="73" t="s">
+      <c r="D84" s="72" t="s">
+        <v>747</v>
+      </c>
+      <c r="E84" s="72" t="s">
+        <v>670</v>
+      </c>
+      <c r="F84" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="G84" s="73" t="s">
-        <v>817</v>
-      </c>
-      <c r="H84" s="73"/>
-      <c r="I84" s="73" t="s">
-        <v>818</v>
-      </c>
-      <c r="J84" s="73" t="s">
+      <c r="G84" s="72" t="s">
+        <v>814</v>
+      </c>
+      <c r="H84" s="72"/>
+      <c r="I84" s="72" t="s">
+        <v>815</v>
+      </c>
+      <c r="J84" s="72" t="s">
         <v>626</v>
       </c>
-      <c r="K84" s="73" t="s">
+      <c r="K84" s="72" t="s">
         <v>626</v>
       </c>
       <c r="L84" s="16" t="s">
@@ -8247,7 +8232,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="19">
+    <row r="85" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A85" s="42" t="s">
         <v>59</v>
       </c>
@@ -8258,7 +8243,7 @@
         <v>461</v>
       </c>
       <c r="D85" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E85" s="43" t="s">
         <v>670</v>
@@ -8289,7 +8274,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="19">
+    <row r="86" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A86" s="42" t="s">
         <v>60</v>
       </c>
@@ -8300,7 +8285,7 @@
         <v>463</v>
       </c>
       <c r="D86" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E86" s="43" t="s">
         <v>670</v>
@@ -8331,7 +8316,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="19">
+    <row r="87" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A87" s="42" t="s">
         <v>260</v>
       </c>
@@ -8342,7 +8327,7 @@
         <v>419</v>
       </c>
       <c r="D87" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E87" s="43" t="s">
         <v>670</v>
@@ -8373,7 +8358,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="19">
+    <row r="88" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A88" s="42" t="s">
         <v>215</v>
       </c>
@@ -8384,7 +8369,7 @@
         <v>315</v>
       </c>
       <c r="D88" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E88" s="43" t="s">
         <v>670</v>
@@ -8415,7 +8400,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="18" customHeight="1">
+    <row r="89" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="42" t="s">
         <v>234</v>
       </c>
@@ -8426,7 +8411,7 @@
         <v>363</v>
       </c>
       <c r="D89" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E89" s="43" t="s">
         <v>670</v>
@@ -8457,7 +8442,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="18" customHeight="1">
+    <row r="90" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="42" t="s">
         <v>222</v>
       </c>
@@ -8468,7 +8453,7 @@
         <v>204</v>
       </c>
       <c r="D90" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E90" s="43" t="s">
         <v>670</v>
@@ -8499,7 +8484,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="18" customHeight="1">
+    <row r="91" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="42" t="s">
         <v>58</v>
       </c>
@@ -8510,7 +8495,7 @@
         <v>458</v>
       </c>
       <c r="D91" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E91" s="43" t="s">
         <v>670</v>
@@ -8541,7 +8526,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="18" customHeight="1">
+    <row r="92" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="42" t="s">
         <v>239</v>
       </c>
@@ -8552,7 +8537,7 @@
         <v>374</v>
       </c>
       <c r="D92" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E92" s="43" t="s">
         <v>670</v>
@@ -8583,7 +8568,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="19">
+    <row r="93" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A93" s="42" t="s">
         <v>233</v>
       </c>
@@ -8594,7 +8579,7 @@
         <v>361</v>
       </c>
       <c r="D93" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E93" s="43" t="s">
         <v>670</v>
@@ -8625,7 +8610,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="19">
+    <row r="94" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
         <v>214</v>
       </c>
@@ -8636,7 +8621,7 @@
         <v>296</v>
       </c>
       <c r="D94" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E94" s="43" t="s">
         <v>670</v>
@@ -8667,7 +8652,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="19">
+    <row r="95" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A95" s="42" t="s">
         <v>61</v>
       </c>
@@ -8678,7 +8663,7 @@
         <v>466</v>
       </c>
       <c r="D95" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E95" s="43" t="s">
         <v>670</v>
@@ -8709,7 +8694,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="19">
+    <row r="96" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="42" t="s">
         <v>271</v>
       </c>
@@ -8720,7 +8705,7 @@
         <v>433</v>
       </c>
       <c r="D96" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E96" s="43" t="s">
         <v>670</v>
@@ -8751,7 +8736,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="19">
+    <row r="97" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="42" t="s">
         <v>220</v>
       </c>
@@ -8762,7 +8747,7 @@
         <v>344</v>
       </c>
       <c r="D97" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E97" s="43" t="s">
         <v>670</v>
@@ -8793,7 +8778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="19">
+    <row r="98" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="42" t="s">
         <v>4</v>
       </c>
@@ -8804,7 +8789,7 @@
         <v>299</v>
       </c>
       <c r="D98" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E98" s="43" t="s">
         <v>670</v>
@@ -8835,7 +8820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="19">
+    <row r="99" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="42" t="s">
         <v>259</v>
       </c>
@@ -8846,7 +8831,7 @@
         <v>417</v>
       </c>
       <c r="D99" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E99" s="43" t="s">
         <v>670</v>
@@ -8877,7 +8862,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="19">
+    <row r="100" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="55" t="s">
         <v>218</v>
       </c>
@@ -8888,7 +8873,7 @@
         <v>335</v>
       </c>
       <c r="D100" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E100" s="57" t="s">
         <v>670</v>
@@ -8919,7 +8904,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="19">
+    <row r="101" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A101" s="55" t="s">
         <v>225</v>
       </c>
@@ -8930,7 +8915,7 @@
         <v>349</v>
       </c>
       <c r="D101" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E101" s="57" t="s">
         <v>670</v>
@@ -8961,7 +8946,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="19">
+    <row r="102" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A102" s="55" t="s">
         <v>227</v>
       </c>
@@ -8972,7 +8957,7 @@
         <v>351</v>
       </c>
       <c r="D102" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E102" s="57" t="s">
         <v>670</v>
@@ -9003,7 +8988,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="19">
+    <row r="103" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A103" s="55" t="s">
         <v>232</v>
       </c>
@@ -9014,7 +8999,7 @@
         <v>594</v>
       </c>
       <c r="D103" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E103" s="57" t="s">
         <v>670</v>
@@ -9045,7 +9030,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="19">
+    <row r="104" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A104" s="55" t="s">
         <v>286</v>
       </c>
@@ -9056,7 +9041,7 @@
         <v>422</v>
       </c>
       <c r="D104" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E104" s="57" t="s">
         <v>670</v>
@@ -9087,7 +9072,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="19">
+    <row r="105" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A105" s="55" t="s">
         <v>258</v>
       </c>
@@ -9098,7 +9083,7 @@
         <v>595</v>
       </c>
       <c r="D105" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E105" s="57" t="s">
         <v>670</v>
@@ -9129,7 +9114,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="19">
+    <row r="106" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A106" s="55" t="s">
         <v>231</v>
       </c>
@@ -9140,7 +9125,7 @@
         <v>598</v>
       </c>
       <c r="D106" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E106" s="57" t="s">
         <v>670</v>
@@ -9171,7 +9156,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="19">
+    <row r="107" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A107" s="55" t="s">
         <v>250</v>
       </c>
@@ -9182,7 +9167,7 @@
         <v>409</v>
       </c>
       <c r="D107" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E107" s="57" t="s">
         <v>670</v>
@@ -9213,7 +9198,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="19">
+    <row r="108" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A108" s="55" t="s">
         <v>253</v>
       </c>
@@ -9224,7 +9209,7 @@
         <v>596</v>
       </c>
       <c r="D108" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E108" s="57" t="s">
         <v>670</v>
@@ -9255,7 +9240,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="19">
+    <row r="109" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A109" s="55" t="s">
         <v>265</v>
       </c>
@@ -9266,7 +9251,7 @@
         <v>597</v>
       </c>
       <c r="D109" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E109" s="57" t="s">
         <v>670</v>
@@ -9297,7 +9282,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="19">
+    <row r="110" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A110" s="55" t="s">
         <v>655</v>
       </c>
@@ -9308,7 +9293,7 @@
         <v>657</v>
       </c>
       <c r="D110" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E110" s="57" t="s">
         <v>670</v>
@@ -9339,7 +9324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="19">
+    <row r="111" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A111" s="55" t="s">
         <v>667</v>
       </c>
@@ -9350,7 +9335,7 @@
         <v>659</v>
       </c>
       <c r="D111" s="57" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E111" s="57" t="s">
         <v>670</v>
@@ -9379,30 +9364,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="19">
+    <row r="112" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A112" s="55" t="s">
         <v>554</v>
       </c>
       <c r="B112" s="56" t="s">
         <v>557</v>
       </c>
-      <c r="C112" s="67" t="s">
+      <c r="C112" s="66" t="s">
         <v>609</v>
       </c>
-      <c r="D112" s="67" t="s">
-        <v>749</v>
-      </c>
-      <c r="E112" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F112" s="67" t="s">
+      <c r="D112" s="66" t="s">
+        <v>747</v>
+      </c>
+      <c r="E112" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F112" s="66" t="s">
         <v>483</v>
       </c>
-      <c r="G112" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H112" s="66"/>
-      <c r="I112" s="66" t="s">
+      <c r="G112" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H112" s="65"/>
+      <c r="I112" s="65" t="s">
         <v>562</v>
       </c>
       <c r="J112" s="14" t="s">
@@ -9421,30 +9406,30 @@
         <v>561</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="19">
+    <row r="113" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A113" s="55" t="s">
         <v>482</v>
       </c>
       <c r="B113" s="56" t="s">
         <v>489</v>
       </c>
-      <c r="C113" s="66" t="s">
+      <c r="C113" s="65" t="s">
         <v>486</v>
       </c>
-      <c r="D113" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E113" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F113" s="67" t="s">
+      <c r="D113" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E113" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F113" s="66" t="s">
         <v>483</v>
       </c>
-      <c r="G113" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H113" s="66"/>
-      <c r="I113" s="66" t="s">
+      <c r="G113" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65" t="s">
         <v>541</v>
       </c>
       <c r="J113" s="14" t="s">
@@ -9463,30 +9448,30 @@
         <v>540</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="19">
+    <row r="114" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A114" s="55" t="s">
         <v>487</v>
       </c>
       <c r="B114" s="56" t="s">
         <v>484</v>
       </c>
-      <c r="C114" s="66" t="s">
+      <c r="C114" s="65" t="s">
         <v>485</v>
       </c>
-      <c r="D114" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E114" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F114" s="67" t="s">
+      <c r="D114" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E114" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F114" s="66" t="s">
         <v>483</v>
       </c>
-      <c r="G114" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H114" s="66"/>
-      <c r="I114" s="66" t="s">
+      <c r="G114" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65" t="s">
         <v>539</v>
       </c>
       <c r="J114" s="14" t="s">
@@ -9505,174 +9490,174 @@
         <v>538</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="19">
+    <row r="115" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A115" s="55" t="s">
         <v>631</v>
       </c>
       <c r="B115" s="56" t="s">
         <v>632</v>
       </c>
-      <c r="C115" s="66" t="s">
+      <c r="C115" s="65" t="s">
+        <v>807</v>
+      </c>
+      <c r="D115" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E115" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F115" s="66" t="s">
+        <v>483</v>
+      </c>
+      <c r="G115" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65" t="s">
+        <v>633</v>
+      </c>
+      <c r="J115" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K115" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L115" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M115" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N115" s="54"/>
+    </row>
+    <row r="116" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A116" s="55" t="s">
+        <v>782</v>
+      </c>
+      <c r="B116" s="56" t="s">
+        <v>783</v>
+      </c>
+      <c r="C116" s="65" t="s">
+        <v>808</v>
+      </c>
+      <c r="D116" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E116" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F116" s="66" t="s">
+        <v>483</v>
+      </c>
+      <c r="G116" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H116" s="65"/>
+      <c r="I116" s="65"/>
+      <c r="J116" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K116" s="14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A117" s="55" t="s">
+        <v>784</v>
+      </c>
+      <c r="B117" s="56" t="s">
+        <v>785</v>
+      </c>
+      <c r="C117" s="65" t="s">
+        <v>806</v>
+      </c>
+      <c r="D117" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E117" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F117" s="66" t="s">
+        <v>483</v>
+      </c>
+      <c r="G117" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H117" s="65"/>
+      <c r="I117" s="65"/>
+      <c r="J117" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K117" s="14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A118" s="55" t="s">
+        <v>788</v>
+      </c>
+      <c r="B118" s="56" t="s">
+        <v>789</v>
+      </c>
+      <c r="C118" s="65" t="s">
+        <v>809</v>
+      </c>
+      <c r="D118" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E118" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F118" s="66" t="s">
+        <v>483</v>
+      </c>
+      <c r="G118" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H118" s="65"/>
+      <c r="I118" s="65"/>
+      <c r="J118" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K118" s="14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="55" t="s">
+        <v>790</v>
+      </c>
+      <c r="B119" s="56" t="s">
+        <v>791</v>
+      </c>
+      <c r="C119" s="65" t="s">
         <v>810</v>
       </c>
-      <c r="D115" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E115" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F115" s="67" t="s">
+      <c r="D119" s="65" t="s">
+        <v>747</v>
+      </c>
+      <c r="E119" s="66" t="s">
+        <v>670</v>
+      </c>
+      <c r="F119" s="66" t="s">
         <v>483</v>
       </c>
-      <c r="G115" s="67" t="s">
+      <c r="G119" s="66" t="s">
+        <v>792</v>
+      </c>
+      <c r="H119" s="65"/>
+      <c r="I119" s="65"/>
+      <c r="J119" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K119" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="N119" s="54" t="s">
         <v>795</v>
       </c>
-      <c r="H115" s="66"/>
-      <c r="I115" s="66" t="s">
-        <v>633</v>
-      </c>
-      <c r="J115" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K115" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L115" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M115" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N115" s="54"/>
-    </row>
-    <row r="116" spans="1:14" ht="19">
-      <c r="A116" s="55" t="s">
-        <v>785</v>
-      </c>
-      <c r="B116" s="56" t="s">
-        <v>786</v>
-      </c>
-      <c r="C116" s="66" t="s">
-        <v>811</v>
-      </c>
-      <c r="D116" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E116" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F116" s="67" t="s">
-        <v>483</v>
-      </c>
-      <c r="G116" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H116" s="66"/>
-      <c r="I116" s="66"/>
-      <c r="J116" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K116" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="19">
-      <c r="A117" s="55" t="s">
-        <v>787</v>
-      </c>
-      <c r="B117" s="56" t="s">
-        <v>788</v>
-      </c>
-      <c r="C117" s="66" t="s">
-        <v>809</v>
-      </c>
-      <c r="D117" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E117" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F117" s="67" t="s">
-        <v>483</v>
-      </c>
-      <c r="G117" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H117" s="66"/>
-      <c r="I117" s="66"/>
-      <c r="J117" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K117" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" ht="19">
-      <c r="A118" s="55" t="s">
-        <v>791</v>
-      </c>
-      <c r="B118" s="56" t="s">
-        <v>792</v>
-      </c>
-      <c r="C118" s="66" t="s">
-        <v>812</v>
-      </c>
-      <c r="D118" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E118" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F118" s="67" t="s">
-        <v>483</v>
-      </c>
-      <c r="G118" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H118" s="66"/>
-      <c r="I118" s="66"/>
-      <c r="J118" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K118" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="119" spans="1:14" ht="19">
-      <c r="A119" s="55" t="s">
-        <v>793</v>
-      </c>
-      <c r="B119" s="56" t="s">
-        <v>794</v>
-      </c>
-      <c r="C119" s="66" t="s">
-        <v>813</v>
-      </c>
-      <c r="D119" s="66" t="s">
-        <v>749</v>
-      </c>
-      <c r="E119" s="67" t="s">
-        <v>670</v>
-      </c>
-      <c r="F119" s="67" t="s">
-        <v>483</v>
-      </c>
-      <c r="G119" s="67" t="s">
-        <v>795</v>
-      </c>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K119" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="N119" s="54" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" ht="19">
+    </row>
+    <row r="120" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A120" s="55" t="s">
         <v>615</v>
       </c>
@@ -9683,7 +9668,7 @@
         <v>610</v>
       </c>
       <c r="D120" s="52" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E120" s="53" t="s">
         <v>670</v>
@@ -9692,7 +9677,7 @@
         <v>483</v>
       </c>
       <c r="G120" s="53" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="H120" s="52"/>
       <c r="I120" s="52" t="s">
@@ -9714,7 +9699,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="19">
+    <row r="121" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A121" s="55" t="s">
         <v>616</v>
       </c>
@@ -9725,7 +9710,7 @@
         <v>671</v>
       </c>
       <c r="D121" s="52" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E121" s="53" t="s">
         <v>670</v>
@@ -9734,7 +9719,7 @@
         <v>483</v>
       </c>
       <c r="G121" s="53" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="H121" s="52"/>
       <c r="I121" s="52" t="s">
@@ -9756,18 +9741,18 @@
         <v>492</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="19">
+    <row r="122" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A122" s="55" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B122" s="56" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="C122" s="52" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="D122" s="52" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E122" s="53" t="s">
         <v>670</v>
@@ -9776,7 +9761,7 @@
         <v>483</v>
       </c>
       <c r="G122" s="53" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="H122" s="52"/>
       <c r="I122" s="52"/>
@@ -9787,18 +9772,18 @@
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="19">
+    <row r="123" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A123" s="55" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B123" s="56" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C123" s="47" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D123" s="47" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E123" s="47" t="s">
         <v>670</v>
@@ -9807,7 +9792,7 @@
         <v>618</v>
       </c>
       <c r="G123" s="47" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="H123" s="47"/>
       <c r="I123" s="47"/>
@@ -9819,18 +9804,18 @@
       </c>
       <c r="L123" s="59"/>
     </row>
-    <row r="124" spans="1:14" ht="19">
+    <row r="124" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A124" s="55" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B124" s="56" t="s">
+        <v>767</v>
+      </c>
+      <c r="C124" s="47" t="s">
         <v>770</v>
       </c>
-      <c r="C124" s="47" t="s">
-        <v>773</v>
-      </c>
       <c r="D124" s="47" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E124" s="47" t="s">
         <v>670</v>
@@ -9839,7 +9824,7 @@
         <v>618</v>
       </c>
       <c r="G124" s="47" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="H124" s="47"/>
       <c r="I124" s="47"/>
@@ -9850,7 +9835,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="19">
+    <row r="125" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A125" s="55" t="s">
         <v>235</v>
       </c>
@@ -9861,7 +9846,7 @@
         <v>366</v>
       </c>
       <c r="D125" s="47" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E125" s="47" t="s">
         <v>670</v>
@@ -9892,7 +9877,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="19">
+    <row r="126" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A126" s="55" t="s">
         <v>497</v>
       </c>
@@ -9903,7 +9888,7 @@
         <v>607</v>
       </c>
       <c r="D126" s="47" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E126" s="47" t="s">
         <v>670</v>
@@ -9932,7 +9917,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="19">
+    <row r="127" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A127" s="55" t="s">
         <v>495</v>
       </c>
@@ -9940,10 +9925,10 @@
         <v>498</v>
       </c>
       <c r="C127" s="47" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="D127" s="47" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E127" s="47" t="s">
         <v>670</v>
@@ -9972,7 +9957,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="19">
+    <row r="128" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A128" s="55" t="s">
         <v>496</v>
       </c>
@@ -9980,10 +9965,10 @@
         <v>499</v>
       </c>
       <c r="C128" s="47" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D128" s="47" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E128" s="47" t="s">
         <v>670</v>
@@ -10012,30 +9997,30 @@
         <v>500</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="18">
+    <row r="129" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A129" s="55" t="s">
         <v>555</v>
       </c>
       <c r="B129" s="56" t="s">
         <v>556</v>
       </c>
-      <c r="C129" s="68" t="s">
+      <c r="C129" s="67" t="s">
         <v>611</v>
       </c>
-      <c r="D129" s="69" t="s">
-        <v>749</v>
-      </c>
-      <c r="E129" s="70" t="s">
-        <v>670</v>
-      </c>
-      <c r="F129" s="70" t="s">
+      <c r="D129" s="68" t="s">
+        <v>747</v>
+      </c>
+      <c r="E129" s="69" t="s">
+        <v>670</v>
+      </c>
+      <c r="F129" s="69" t="s">
         <v>483</v>
       </c>
-      <c r="G129" s="70" t="s">
-        <v>797</v>
-      </c>
-      <c r="H129" s="68"/>
-      <c r="I129" s="68" t="s">
+      <c r="G129" s="69" t="s">
+        <v>794</v>
+      </c>
+      <c r="H129" s="67"/>
+      <c r="I129" s="67" t="s">
         <v>564</v>
       </c>
       <c r="J129" s="14" t="s">
@@ -10054,30 +10039,30 @@
         <v>563</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="18">
+    <row r="130" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A130" s="55" t="s">
         <v>553</v>
       </c>
       <c r="B130" s="56" t="s">
         <v>558</v>
       </c>
-      <c r="C130" s="68" t="s">
+      <c r="C130" s="67" t="s">
         <v>608</v>
       </c>
-      <c r="D130" s="69" t="s">
-        <v>749</v>
-      </c>
-      <c r="E130" s="70" t="s">
-        <v>670</v>
-      </c>
-      <c r="F130" s="70" t="s">
+      <c r="D130" s="68" t="s">
+        <v>747</v>
+      </c>
+      <c r="E130" s="69" t="s">
+        <v>670</v>
+      </c>
+      <c r="F130" s="69" t="s">
         <v>483</v>
       </c>
-      <c r="G130" s="70" t="s">
-        <v>797</v>
-      </c>
-      <c r="H130" s="68"/>
-      <c r="I130" s="68" t="s">
+      <c r="G130" s="69" t="s">
+        <v>794</v>
+      </c>
+      <c r="H130" s="67"/>
+      <c r="I130" s="67" t="s">
         <v>560</v>
       </c>
       <c r="J130" s="14" t="s">
@@ -10096,7 +10081,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="19">
+    <row r="131" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A131" s="27" t="s">
         <v>236</v>
       </c>
@@ -10107,10 +10092,10 @@
         <v>207</v>
       </c>
       <c r="D131" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F131" s="26" t="s">
         <v>368</v>
@@ -10136,7 +10121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="19">
+    <row r="132" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A132" s="27" t="s">
         <v>270</v>
       </c>
@@ -10147,10 +10132,10 @@
         <v>590</v>
       </c>
       <c r="D132" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E132" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F132" s="26" t="s">
         <v>368</v>
@@ -10176,7 +10161,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="19">
+    <row r="133" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A133" s="27" t="s">
         <v>262</v>
       </c>
@@ -10187,10 +10172,10 @@
         <v>591</v>
       </c>
       <c r="D133" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E133" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F133" s="26" t="s">
         <v>368</v>
@@ -10216,7 +10201,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="19">
+    <row r="134" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A134" s="27" t="s">
         <v>263</v>
       </c>
@@ -10227,10 +10212,10 @@
         <v>592</v>
       </c>
       <c r="D134" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E134" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F134" s="26" t="s">
         <v>368</v>
@@ -10256,7 +10241,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="19">
+    <row r="135" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A135" s="27" t="s">
         <v>264</v>
       </c>
@@ -10267,10 +10252,10 @@
         <v>593</v>
       </c>
       <c r="D135" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E135" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F135" s="26" t="s">
         <v>368</v>
@@ -10296,7 +10281,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="19">
+    <row r="136" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A136" s="27" t="s">
         <v>256</v>
       </c>
@@ -10307,10 +10292,10 @@
         <v>32</v>
       </c>
       <c r="D136" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E136" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F136" s="26" t="s">
         <v>368</v>
@@ -10336,9 +10321,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="19">
+    <row r="137" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A137" s="27" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B137" s="28" t="s">
         <v>147</v>
@@ -10347,10 +10332,10 @@
         <v>672</v>
       </c>
       <c r="D137" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F137" s="28" t="s">
         <v>368</v>
@@ -10358,7 +10343,7 @@
       <c r="G137" s="28"/>
       <c r="H137" s="28"/>
       <c r="I137" s="28" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J137" s="14" t="s">
         <v>197</v>
@@ -10367,27 +10352,27 @@
         <v>197</v>
       </c>
       <c r="L137" s="59" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="M137" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="19">
+    <row r="138" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A138" s="27" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B138" s="28" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C138" s="28" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D138" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E138" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F138" s="28" t="s">
         <v>368</v>
@@ -10395,7 +10380,7 @@
       <c r="G138" s="28"/>
       <c r="H138" s="28"/>
       <c r="I138" s="28" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="J138" s="14" t="s">
         <v>197</v>
@@ -10404,27 +10389,27 @@
         <v>197</v>
       </c>
       <c r="L138" s="59" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="M138" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="19">
+    <row r="139" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A139" s="27" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B139" s="28" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C139" s="28" t="s">
+        <v>756</v>
+      </c>
+      <c r="D139" s="26" t="s">
+        <v>747</v>
+      </c>
+      <c r="E139" s="26" t="s">
         <v>758</v>
-      </c>
-      <c r="D139" s="26" t="s">
-        <v>749</v>
-      </c>
-      <c r="E139" s="26" t="s">
-        <v>760</v>
       </c>
       <c r="F139" s="28" t="s">
         <v>368</v>
@@ -10432,36 +10417,36 @@
       <c r="G139" s="28"/>
       <c r="H139" s="28"/>
       <c r="I139" s="28" t="s">
+        <v>725</v>
+      </c>
+      <c r="J139" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K139" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L139" s="59" t="s">
+        <v>726</v>
+      </c>
+      <c r="M139" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A140" s="27" t="s">
+        <v>679</v>
+      </c>
+      <c r="B140" s="28" t="s">
         <v>727</v>
       </c>
-      <c r="J139" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K139" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L139" s="59" t="s">
-        <v>728</v>
-      </c>
-      <c r="M139" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" ht="19">
-      <c r="A140" s="27" t="s">
-        <v>681</v>
-      </c>
-      <c r="B140" s="28" t="s">
-        <v>729</v>
-      </c>
       <c r="C140" s="28" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D140" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E140" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F140" s="28" t="s">
         <v>368</v>
@@ -10469,7 +10454,7 @@
       <c r="G140" s="28"/>
       <c r="H140" s="28"/>
       <c r="I140" s="28" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="J140" s="14" t="s">
         <v>197</v>
@@ -10484,21 +10469,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="19">
+    <row r="141" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A141" s="27" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B141" s="28" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C141" s="28" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D141" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E141" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F141" s="28" t="s">
         <v>368</v>
@@ -10506,7 +10491,7 @@
       <c r="G141" s="28"/>
       <c r="H141" s="28"/>
       <c r="I141" s="28" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="J141" s="14" t="s">
         <v>197</v>
@@ -10515,27 +10500,27 @@
         <v>197</v>
       </c>
       <c r="L141" s="59" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="M141" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="19">
+    <row r="142" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A142" s="27" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B142" s="28" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C142" s="28" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D142" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E142" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F142" s="28" t="s">
         <v>368</v>
@@ -10543,7 +10528,7 @@
       <c r="G142" s="28"/>
       <c r="H142" s="28"/>
       <c r="I142" s="28" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="J142" s="14" t="s">
         <v>197</v>
@@ -10552,27 +10537,27 @@
         <v>197</v>
       </c>
       <c r="L142" s="59" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="M142" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="19">
+    <row r="143" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A143" s="27" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B143" s="28" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C143" s="28" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D143" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E143" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F143" s="28" t="s">
         <v>368</v>
@@ -10580,7 +10565,7 @@
       <c r="G143" s="28"/>
       <c r="H143" s="28"/>
       <c r="I143" s="28" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="J143" s="14" t="s">
         <v>197</v>
@@ -10589,27 +10574,27 @@
         <v>197</v>
       </c>
       <c r="L143" s="59" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="M143" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="19">
+    <row r="144" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A144" s="27" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B144" s="28" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C144" s="28" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D144" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E144" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F144" s="28" t="s">
         <v>368</v>
@@ -10617,7 +10602,7 @@
       <c r="G144" s="28"/>
       <c r="H144" s="28"/>
       <c r="I144" s="28" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="J144" s="14" t="s">
         <v>197</v>
@@ -10626,34 +10611,34 @@
         <v>197</v>
       </c>
       <c r="L144" s="59" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M144" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="19">
+    <row r="145" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A145" s="27" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B145" s="28" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C145" s="28" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D145" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E145" s="26" t="s">
-        <v>760</v>
-      </c>
-      <c r="F145" s="63" t="s">
-        <v>761</v>
-      </c>
-      <c r="G145" s="63"/>
-      <c r="H145" s="63"/>
-      <c r="I145" s="63" t="s">
+        <v>758</v>
+      </c>
+      <c r="F145" s="58" t="s">
+        <v>416</v>
+      </c>
+      <c r="G145" s="58"/>
+      <c r="H145" s="58"/>
+      <c r="I145" s="58" t="s">
         <v>119</v>
       </c>
       <c r="J145" s="39" t="s">
@@ -10663,7 +10648,7 @@
         <v>197</v>
       </c>
       <c r="L145" s="59" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="M145" s="58" t="s">
         <v>1</v>
@@ -10672,7 +10657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="19">
+    <row r="146" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A146" s="27" t="s">
         <v>254</v>
       </c>
@@ -10683,10 +10668,10 @@
         <v>602</v>
       </c>
       <c r="D146" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E146" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F146" s="58" t="s">
         <v>416</v>
@@ -10712,7 +10697,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="19">
+    <row r="147" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A147" s="27" t="s">
         <v>221</v>
       </c>
@@ -10723,10 +10708,10 @@
         <v>346</v>
       </c>
       <c r="D147" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E147" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F147" s="39" t="s">
         <v>416</v>
@@ -10752,7 +10737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="19">
+    <row r="148" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A148" s="27" t="s">
         <v>287</v>
       </c>
@@ -10763,10 +10748,10 @@
         <v>437</v>
       </c>
       <c r="D148" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E148" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F148" s="58" t="s">
         <v>416</v>
@@ -10792,7 +10777,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="19">
+    <row r="149" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A149" s="27" t="s">
         <v>266</v>
       </c>
@@ -10803,10 +10788,10 @@
         <v>601</v>
       </c>
       <c r="D149" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E149" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F149" s="39" t="s">
         <v>416</v>
@@ -10832,7 +10817,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="19">
+    <row r="150" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A150" s="27" t="s">
         <v>223</v>
       </c>
@@ -10843,10 +10828,10 @@
         <v>348</v>
       </c>
       <c r="D150" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E150" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F150" s="39" t="s">
         <v>416</v>
@@ -10872,7 +10857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="19">
+    <row r="151" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A151" s="27" t="s">
         <v>257</v>
       </c>
@@ -10883,10 +10868,10 @@
         <v>600</v>
       </c>
       <c r="D151" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E151" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F151" s="39" t="s">
         <v>416</v>
@@ -10912,7 +10897,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="19">
+    <row r="152" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A152" s="27" t="s">
         <v>261</v>
       </c>
@@ -10923,10 +10908,10 @@
         <v>599</v>
       </c>
       <c r="D152" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E152" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F152" s="39" t="s">
         <v>416</v>
@@ -10952,21 +10937,21 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="19">
+    <row r="153" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A153" s="27" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B153" s="28" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C153" s="28" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D153" s="26" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E153" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F153" s="39" t="s">
         <v>416</v>
@@ -10974,7 +10959,7 @@
       <c r="G153" s="39"/>
       <c r="H153" s="39"/>
       <c r="I153" s="39" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="J153" s="39" t="s">
         <v>197</v>
@@ -10989,34 +10974,32 @@
         <v>1</v>
       </c>
       <c r="N153" s="16" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="154" spans="1:14" ht="19">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A154" s="48" t="s">
-        <v>570</v>
+        <v>818</v>
       </c>
       <c r="B154" s="49" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="C154" s="49" t="s">
-        <v>605</v>
+        <v>818</v>
       </c>
       <c r="D154" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E154" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F154" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G154" s="49" t="s">
         <v>673</v>
       </c>
-      <c r="H154" s="49">
-        <v>1</v>
-      </c>
+      <c r="H154" s="49"/>
       <c r="I154" s="49" t="s">
         <v>519</v>
       </c>
@@ -11024,7 +11007,7 @@
         <v>647</v>
       </c>
       <c r="K154" s="14" t="s">
-        <v>197</v>
+        <v>630</v>
       </c>
       <c r="L154" s="15" t="s">
         <v>666</v>
@@ -11036,24 +11019,24 @@
         <v>583</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="19">
+    <row r="155" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A155" s="48" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B155" s="49" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C155" s="49" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D155" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E155" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F155" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G155" s="49" t="s">
         <v>673</v>
@@ -11062,42 +11045,42 @@
         <v>1</v>
       </c>
       <c r="I155" s="49" t="s">
-        <v>578</v>
+        <v>519</v>
       </c>
       <c r="J155" s="14" t="s">
-        <v>197</v>
+        <v>647</v>
       </c>
       <c r="K155" s="14" t="s">
-        <v>197</v>
+        <v>630</v>
       </c>
       <c r="L155" s="15" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="M155" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N155" s="16" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="156" spans="1:14" ht="19">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A156" s="48" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B156" s="49" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C156" s="49" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D156" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E156" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F156" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G156" s="49" t="s">
         <v>673</v>
@@ -11106,7 +11089,7 @@
         <v>1</v>
       </c>
       <c r="I156" s="49" t="s">
-        <v>403</v>
+        <v>578</v>
       </c>
       <c r="J156" s="14" t="s">
         <v>197</v>
@@ -11115,33 +11098,33 @@
         <v>197</v>
       </c>
       <c r="L156" s="15" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="M156" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N156" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="157" spans="1:14" ht="19">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A157" s="48" t="s">
-        <v>661</v>
+        <v>567</v>
       </c>
       <c r="B157" s="49" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C157" s="49" t="s">
-        <v>572</v>
+        <v>603</v>
       </c>
       <c r="D157" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E157" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F157" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G157" s="49" t="s">
         <v>673</v>
@@ -11150,42 +11133,42 @@
         <v>1</v>
       </c>
       <c r="I157" s="49" t="s">
-        <v>520</v>
+        <v>403</v>
       </c>
       <c r="J157" s="14" t="s">
-        <v>647</v>
+        <v>197</v>
       </c>
       <c r="K157" s="14" t="s">
         <v>197</v>
       </c>
       <c r="L157" s="15" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="M157" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N157" s="16" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" ht="19">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="48" t="s">
-        <v>569</v>
+        <v>661</v>
       </c>
       <c r="B158" s="49" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C158" s="49" t="s">
-        <v>606</v>
+        <v>572</v>
       </c>
       <c r="D158" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E158" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F158" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G158" s="49" t="s">
         <v>673</v>
@@ -11194,42 +11177,42 @@
         <v>1</v>
       </c>
       <c r="I158" s="49" t="s">
-        <v>580</v>
+        <v>520</v>
       </c>
       <c r="J158" s="14" t="s">
-        <v>197</v>
+        <v>647</v>
       </c>
       <c r="K158" s="14" t="s">
-        <v>197</v>
+        <v>630</v>
       </c>
       <c r="L158" s="15" t="s">
-        <v>1</v>
+        <v>663</v>
       </c>
       <c r="M158" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N158" s="16" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" ht="19">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="48" t="s">
-        <v>635</v>
+        <v>569</v>
       </c>
       <c r="B159" s="49" t="s">
-        <v>636</v>
+        <v>575</v>
       </c>
       <c r="C159" s="49" t="s">
-        <v>652</v>
+        <v>606</v>
       </c>
       <c r="D159" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E159" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F159" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G159" s="49" t="s">
         <v>673</v>
@@ -11238,7 +11221,7 @@
         <v>1</v>
       </c>
       <c r="I159" s="49" t="s">
-        <v>651</v>
+        <v>580</v>
       </c>
       <c r="J159" s="14" t="s">
         <v>197</v>
@@ -11253,27 +11236,27 @@
         <v>1</v>
       </c>
       <c r="N159" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:14" ht="19">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="48" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B160" s="49" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C160" s="49" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D160" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E160" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F160" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G160" s="49" t="s">
         <v>673</v>
@@ -11282,7 +11265,7 @@
         <v>1</v>
       </c>
       <c r="I160" s="49" t="s">
-        <v>677</v>
+        <v>651</v>
       </c>
       <c r="J160" s="14" t="s">
         <v>197</v>
@@ -11300,118 +11283,121 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="19">
+    <row r="161" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="48" t="s">
+        <v>638</v>
+      </c>
+      <c r="B161" s="49" t="s">
+        <v>637</v>
+      </c>
+      <c r="C161" s="49" t="s">
+        <v>653</v>
+      </c>
+      <c r="D161" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="E161" s="49" t="s">
+        <v>670</v>
+      </c>
+      <c r="F161" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="G161" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="H161" s="49">
+        <v>1</v>
+      </c>
+      <c r="I161" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="J161" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K161" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L161" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M161" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N161" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A162" s="48" t="s">
         <v>662</v>
       </c>
-      <c r="B161" s="49" t="s">
+      <c r="B162" s="49" t="s">
         <v>571</v>
       </c>
-      <c r="C161" s="49" t="s">
+      <c r="C162" s="49" t="s">
         <v>572</v>
       </c>
-      <c r="D161" s="49" t="s">
-        <v>675</v>
-      </c>
-      <c r="E161" s="49" t="s">
-        <v>670</v>
-      </c>
-      <c r="F161" s="49" t="s">
-        <v>675</v>
-      </c>
-      <c r="G161" s="49" t="s">
-        <v>674</v>
-      </c>
-      <c r="H161" s="49">
-        <v>3</v>
-      </c>
-      <c r="I161" s="49" t="s">
-        <v>520</v>
-      </c>
-      <c r="J161" s="14" t="s">
-        <v>647</v>
-      </c>
-      <c r="K161" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L161" s="15" t="s">
-        <v>663</v>
-      </c>
-      <c r="M161" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="N161" s="16" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" ht="19">
-      <c r="A162" s="48" t="s">
-        <v>814</v>
-      </c>
-      <c r="B162" s="49" t="s">
-        <v>574</v>
-      </c>
-      <c r="C162" s="49" t="s">
-        <v>604</v>
-      </c>
       <c r="D162" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E162" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F162" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G162" s="49" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H162" s="49">
         <v>3</v>
       </c>
       <c r="I162" s="49" t="s">
-        <v>578</v>
+        <v>520</v>
       </c>
       <c r="J162" s="14" t="s">
-        <v>197</v>
+        <v>647</v>
       </c>
       <c r="K162" s="14" t="s">
-        <v>197</v>
+        <v>630</v>
       </c>
       <c r="L162" s="15" t="s">
-        <v>665</v>
+        <v>663</v>
+      </c>
+      <c r="M162" s="50" t="s">
+        <v>1</v>
       </c>
       <c r="N162" s="16" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" ht="19">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="48" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B163" s="49" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C163" s="49" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D163" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E163" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F163" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G163" s="49" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H163" s="49">
         <v>3</v>
       </c>
       <c r="I163" s="49" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J163" s="14" t="s">
         <v>197</v>
@@ -11420,65 +11406,106 @@
         <v>197</v>
       </c>
       <c r="L163" s="15" t="s">
-        <v>1</v>
+        <v>665</v>
       </c>
       <c r="N163" s="16" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" ht="19">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A164" s="48" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B164" s="49" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C164" s="49" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D164" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E164" s="49" t="s">
         <v>670</v>
       </c>
       <c r="F164" s="49" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G164" s="49" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H164" s="49">
         <v>3</v>
       </c>
       <c r="I164" s="49" t="s">
+        <v>580</v>
+      </c>
+      <c r="J164" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K164" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L164" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N164" s="16" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A165" s="48" t="s">
+        <v>813</v>
+      </c>
+      <c r="B165" s="49" t="s">
+        <v>573</v>
+      </c>
+      <c r="C165" s="49" t="s">
+        <v>603</v>
+      </c>
+      <c r="D165" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="E165" s="49" t="s">
+        <v>670</v>
+      </c>
+      <c r="F165" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="G165" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="H165" s="49">
+        <v>3</v>
+      </c>
+      <c r="I165" s="49" t="s">
         <v>403</v>
       </c>
-      <c r="J164" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="K164" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="L164" s="15" t="s">
+      <c r="J165" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="K165" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L165" s="15" t="s">
         <v>664</v>
       </c>
-      <c r="N164" s="16" t="s">
+      <c r="N165" s="16" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="165" spans="1:14">
-      <c r="A165" s="1"/>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A166" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:N161">
-    <sortCondition ref="D2:D161"/>
-    <sortCondition ref="E2:E161"/>
-    <sortCondition ref="F2:F161"/>
-    <sortCondition ref="G2:G161"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N162">
+    <sortCondition ref="D2:D162"/>
+    <sortCondition ref="E2:E162"/>
+    <sortCondition ref="F2:F162"/>
+    <sortCondition ref="G2:G162"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B61" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus"/>
+    <hyperlink ref="B61" r:id="rId1" display="https://it.wikipedia.org/wiki/Baiyangdian_virus" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11491,16 +11518,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1">
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>617</v>
       </c>
@@ -11532,7 +11559,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="19">
+    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>242</v>
       </c>
@@ -11543,7 +11570,7 @@
         <v>380</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E2" s="43" t="s">
         <v>670</v>

</xml_diff>

<commit_message>
Added more dISF clades as alignments with residues
</commit_message>
<xml_diff>
--- a/tabular/virus/flavi-ncbi-refseqs-side-data.xlsx
+++ b/tabular/virus/flavi-ncbi-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/virus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/virus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE21B36-76C7-AD40-9B38-C4CC0C61C4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A13A50-6897-9440-A651-E2AA8D3C90AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="34680" windowHeight="20940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4693,8 +4693,8 @@
   <dimension ref="A1:N166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>